<commit_message>
chargebacks turned in to GI
7/22/16 entries are guesses
</commit_message>
<xml_diff>
--- a/20160620/Chargebacks Lori 20160620 to 20160722.xlsx
+++ b/20160620/Chargebacks Lori 20160620 to 20160722.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laughreyl\Documents\GitHub\chargebacks\20160620\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laughreyl\Documents\chargebacks\20160620\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43620" yWindow="10635" windowWidth="25125" windowHeight="18540" tabRatio="500"/>
+    <workbookView xWindow="44790" yWindow="10635" windowWidth="25125" windowHeight="18540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oct '15 Lori" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="130">
   <si>
     <t>Summary of hours worked - PTR/Behavior Team</t>
   </si>
@@ -404,12 +404,19 @@
   <si>
     <t>7.75 hours sorting out image locations&amp; renaming</t>
   </si>
+  <si>
+    <t>Keleman</t>
+  </si>
+  <si>
+    <t>Krystyna</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
@@ -1111,8 +1118,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="360">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1666,9 +1674,6 @@
     <xf numFmtId="0" fontId="14" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1757,6 +1762,30 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1805,32 +1834,12 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="43" fontId="14" fillId="17" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2175,8 +2184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G96" sqref="G96"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="L138" sqref="L138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2205,12 +2214,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="338" t="s">
+      <c r="A1" s="345" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="338"/>
-      <c r="C1" s="338"/>
-      <c r="D1" s="338"/>
+      <c r="B1" s="345"/>
+      <c r="C1" s="345"/>
+      <c r="D1" s="345"/>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2218,140 +2227,140 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="L1" s="359" t="s">
+      <c r="L1" s="336" t="s">
         <v>123</v>
       </c>
-      <c r="M1" s="359"/>
-      <c r="N1" s="359"/>
-      <c r="O1" s="359"/>
-      <c r="P1" s="314">
+      <c r="M1" s="336"/>
+      <c r="N1" s="336"/>
+      <c r="O1" s="336"/>
+      <c r="P1" s="313">
         <v>42541</v>
       </c>
-      <c r="Q1" s="315">
+      <c r="Q1" s="314">
         <f>P1+1</f>
         <v>42542</v>
       </c>
-      <c r="R1" s="315">
+      <c r="R1" s="314">
         <f t="shared" ref="R1:AV1" si="0">Q1+1</f>
         <v>42543</v>
       </c>
-      <c r="S1" s="315">
+      <c r="S1" s="314">
         <f t="shared" si="0"/>
         <v>42544</v>
       </c>
-      <c r="T1" s="315">
+      <c r="T1" s="314">
         <f t="shared" si="0"/>
         <v>42545</v>
       </c>
-      <c r="U1" s="315">
+      <c r="U1" s="314">
         <f t="shared" si="0"/>
         <v>42546</v>
       </c>
-      <c r="V1" s="315">
+      <c r="V1" s="314">
         <f t="shared" si="0"/>
         <v>42547</v>
       </c>
-      <c r="W1" s="315">
+      <c r="W1" s="314">
         <f t="shared" si="0"/>
         <v>42548</v>
       </c>
-      <c r="X1" s="315">
+      <c r="X1" s="314">
         <f t="shared" si="0"/>
         <v>42549</v>
       </c>
-      <c r="Y1" s="315">
+      <c r="Y1" s="314">
         <f t="shared" si="0"/>
         <v>42550</v>
       </c>
-      <c r="Z1" s="315">
+      <c r="Z1" s="314">
         <f t="shared" si="0"/>
         <v>42551</v>
       </c>
-      <c r="AA1" s="315">
+      <c r="AA1" s="314">
         <f t="shared" si="0"/>
         <v>42552</v>
       </c>
-      <c r="AB1" s="315">
+      <c r="AB1" s="314">
         <f t="shared" si="0"/>
         <v>42553</v>
       </c>
-      <c r="AC1" s="315">
+      <c r="AC1" s="314">
         <f t="shared" si="0"/>
         <v>42554</v>
       </c>
-      <c r="AD1" s="315">
+      <c r="AD1" s="314">
         <f t="shared" si="0"/>
         <v>42555</v>
       </c>
-      <c r="AE1" s="315">
+      <c r="AE1" s="314">
         <f t="shared" si="0"/>
         <v>42556</v>
       </c>
-      <c r="AF1" s="315">
+      <c r="AF1" s="314">
         <f t="shared" si="0"/>
         <v>42557</v>
       </c>
-      <c r="AG1" s="315">
+      <c r="AG1" s="314">
         <f t="shared" si="0"/>
         <v>42558</v>
       </c>
-      <c r="AH1" s="315">
+      <c r="AH1" s="314">
         <f t="shared" si="0"/>
         <v>42559</v>
       </c>
-      <c r="AI1" s="315">
+      <c r="AI1" s="314">
         <f t="shared" si="0"/>
         <v>42560</v>
       </c>
-      <c r="AJ1" s="335">
+      <c r="AJ1" s="334">
         <f t="shared" si="0"/>
         <v>42561</v>
       </c>
-      <c r="AK1" s="315">
+      <c r="AK1" s="314">
         <f t="shared" si="0"/>
         <v>42562</v>
       </c>
-      <c r="AL1" s="315">
+      <c r="AL1" s="314">
         <f t="shared" si="0"/>
         <v>42563</v>
       </c>
-      <c r="AM1" s="315">
+      <c r="AM1" s="314">
         <f t="shared" si="0"/>
         <v>42564</v>
       </c>
-      <c r="AN1" s="315">
+      <c r="AN1" s="314">
         <f t="shared" si="0"/>
         <v>42565</v>
       </c>
-      <c r="AO1" s="315">
+      <c r="AO1" s="314">
         <f t="shared" si="0"/>
         <v>42566</v>
       </c>
-      <c r="AP1" s="315">
+      <c r="AP1" s="314">
         <f t="shared" si="0"/>
         <v>42567</v>
       </c>
-      <c r="AQ1" s="315">
+      <c r="AQ1" s="314">
         <f t="shared" si="0"/>
         <v>42568</v>
       </c>
-      <c r="AR1" s="315">
+      <c r="AR1" s="314">
         <f t="shared" si="0"/>
         <v>42569</v>
       </c>
-      <c r="AS1" s="315">
+      <c r="AS1" s="314">
         <f t="shared" si="0"/>
         <v>42570</v>
       </c>
-      <c r="AT1" s="315">
+      <c r="AT1" s="314">
         <f t="shared" si="0"/>
         <v>42571</v>
       </c>
-      <c r="AU1" s="315">
+      <c r="AU1" s="314">
         <f t="shared" si="0"/>
         <v>42572</v>
       </c>
-      <c r="AV1" s="315">
+      <c r="AV1" s="314">
         <f t="shared" si="0"/>
         <v>42573</v>
       </c>
@@ -2359,68 +2368,68 @@
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="M2" s="110"/>
       <c r="N2" s="111"/>
-      <c r="O2" s="316" t="s">
+      <c r="O2" s="315" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="355" t="s">
+      <c r="P2" s="340" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="356"/>
-      <c r="R2" s="356"/>
-      <c r="S2" s="356"/>
-      <c r="T2" s="357"/>
+      <c r="Q2" s="341"/>
+      <c r="R2" s="341"/>
+      <c r="S2" s="341"/>
+      <c r="T2" s="342"/>
       <c r="U2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="V2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="W2" s="355" t="s">
+      <c r="W2" s="340" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="356"/>
-      <c r="Y2" s="356"/>
-      <c r="Z2" s="356"/>
-      <c r="AA2" s="357"/>
+      <c r="X2" s="341"/>
+      <c r="Y2" s="341"/>
+      <c r="Z2" s="341"/>
+      <c r="AA2" s="342"/>
       <c r="AB2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="AC2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AD2" s="355" t="s">
+      <c r="AD2" s="340" t="s">
         <v>2</v>
       </c>
-      <c r="AE2" s="356"/>
-      <c r="AF2" s="356"/>
-      <c r="AG2" s="356"/>
-      <c r="AH2" s="357"/>
+      <c r="AE2" s="341"/>
+      <c r="AF2" s="341"/>
+      <c r="AG2" s="341"/>
+      <c r="AH2" s="342"/>
       <c r="AI2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="AJ2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AK2" s="355" t="s">
+      <c r="AK2" s="340" t="s">
         <v>2</v>
       </c>
-      <c r="AL2" s="356"/>
-      <c r="AM2" s="356"/>
-      <c r="AN2" s="356"/>
-      <c r="AO2" s="357"/>
+      <c r="AL2" s="341"/>
+      <c r="AM2" s="341"/>
+      <c r="AN2" s="341"/>
+      <c r="AO2" s="342"/>
       <c r="AP2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="AQ2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AR2" s="355" t="s">
+      <c r="AR2" s="340" t="s">
         <v>2</v>
       </c>
-      <c r="AS2" s="356"/>
-      <c r="AT2" s="356"/>
-      <c r="AU2" s="356"/>
-      <c r="AV2" s="357"/>
+      <c r="AS2" s="341"/>
+      <c r="AT2" s="341"/>
+      <c r="AU2" s="341"/>
+      <c r="AV2" s="342"/>
       <c r="AW2" s="5" t="s">
         <v>3</v>
       </c>
@@ -2445,7 +2454,7 @@
       <c r="H3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="313" t="s">
+      <c r="I3" s="312" t="s">
         <v>6</v>
       </c>
       <c r="J3" s="12" t="s">
@@ -2455,57 +2464,57 @@
       <c r="M3" s="13"/>
       <c r="N3" s="14"/>
       <c r="O3" s="10"/>
-      <c r="P3" s="352" t="s">
+      <c r="P3" s="337" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="353"/>
-      <c r="R3" s="353"/>
-      <c r="S3" s="353"/>
-      <c r="T3" s="354"/>
+      <c r="Q3" s="338"/>
+      <c r="R3" s="338"/>
+      <c r="S3" s="338"/>
+      <c r="T3" s="339"/>
       <c r="U3" s="15" t="s">
         <v>9</v>
       </c>
       <c r="V3" s="16"/>
-      <c r="W3" s="352" t="s">
+      <c r="W3" s="337" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="353"/>
-      <c r="Y3" s="353"/>
-      <c r="Z3" s="353"/>
-      <c r="AA3" s="354"/>
+      <c r="X3" s="338"/>
+      <c r="Y3" s="338"/>
+      <c r="Z3" s="338"/>
+      <c r="AA3" s="339"/>
       <c r="AB3" s="15" t="s">
         <v>9</v>
       </c>
       <c r="AC3" s="16"/>
-      <c r="AD3" s="352" t="s">
+      <c r="AD3" s="337" t="s">
         <v>11</v>
       </c>
-      <c r="AE3" s="353"/>
-      <c r="AF3" s="353"/>
-      <c r="AG3" s="353"/>
-      <c r="AH3" s="354"/>
+      <c r="AE3" s="338"/>
+      <c r="AF3" s="338"/>
+      <c r="AG3" s="338"/>
+      <c r="AH3" s="339"/>
       <c r="AI3" s="15" t="s">
         <v>9</v>
       </c>
       <c r="AJ3" s="16"/>
-      <c r="AK3" s="352" t="s">
+      <c r="AK3" s="337" t="s">
         <v>12</v>
       </c>
-      <c r="AL3" s="353"/>
-      <c r="AM3" s="353"/>
-      <c r="AN3" s="353"/>
-      <c r="AO3" s="354"/>
+      <c r="AL3" s="338"/>
+      <c r="AM3" s="338"/>
+      <c r="AN3" s="338"/>
+      <c r="AO3" s="339"/>
       <c r="AP3" s="15" t="s">
         <v>9</v>
       </c>
       <c r="AQ3" s="16"/>
-      <c r="AR3" s="352" t="s">
+      <c r="AR3" s="337" t="s">
         <v>13</v>
       </c>
-      <c r="AS3" s="353"/>
-      <c r="AT3" s="353"/>
-      <c r="AU3" s="353"/>
-      <c r="AV3" s="354"/>
+      <c r="AS3" s="338"/>
+      <c r="AT3" s="338"/>
+      <c r="AU3" s="338"/>
+      <c r="AV3" s="339"/>
       <c r="AW3" s="17" t="s">
         <v>6</v>
       </c>
@@ -2516,33 +2525,33 @@
       <c r="AZ3" s="14"/>
     </row>
     <row r="4" spans="1:52" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="346" t="s">
+      <c r="A4" s="353" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="347"/>
+      <c r="B4" s="354"/>
       <c r="C4" s="19" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="358" t="str">
+      <c r="E4" s="335" t="str">
         <f>CONCATENATE(TEXT(P1,"MM/DD"),"-",TEXT(T1,"MM/DD"))</f>
         <v>06/20-06/24</v>
       </c>
-      <c r="F4" s="358" t="str">
+      <c r="F4" s="335" t="str">
         <f>CONCATENATE(TEXT(W1,"MM/DD"),"-",TEXT(AA1,"MM/DD"))</f>
         <v>06/27-07/01</v>
       </c>
-      <c r="G4" s="358" t="str">
+      <c r="G4" s="335" t="str">
         <f>CONCATENATE(TEXT(AD1,"MM/DD"),"-",TEXT(AH1,"MM/DD"))</f>
         <v>07/04-07/08</v>
       </c>
-      <c r="H4" s="358" t="str">
+      <c r="H4" s="335" t="str">
         <f>CONCATENATE(TEXT(AK1,"MM/DD"),"-",TEXT(AO1,"MM/DD"))</f>
         <v>07/11-07/15</v>
       </c>
-      <c r="I4" s="358" t="str">
+      <c r="I4" s="335" t="str">
         <f>CONCATENATE(TEXT(AR1,"MM/DD"),"-",TEXT(AV1,"MM/DD"))</f>
         <v>07/18-07/22</v>
       </c>
@@ -2765,10 +2774,10 @@
       <c r="AV6" s="43"/>
       <c r="AW6" s="49"/>
       <c r="AX6" s="50"/>
-      <c r="AY6" s="348" t="s">
+      <c r="AY6" s="355" t="s">
         <v>27</v>
       </c>
-      <c r="AZ6" s="349"/>
+      <c r="AZ6" s="356"/>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
@@ -4311,11 +4320,11 @@
       </c>
       <c r="I20" s="55">
         <f>AW20</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="J20" s="56">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="K20" s="68"/>
       <c r="L20" s="58"/>
@@ -4386,15 +4395,17 @@
       <c r="AR20" s="86"/>
       <c r="AS20" s="55"/>
       <c r="AT20" s="55"/>
-      <c r="AU20" s="55"/>
+      <c r="AU20" s="55">
+        <v>0.25</v>
+      </c>
       <c r="AV20" s="55"/>
       <c r="AW20" s="64">
         <f>SUM(AR20:AV20)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AX20" s="65">
         <f>U20+AB20+AI20+AP20+AW20</f>
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="AY20" s="66" t="s">
         <v>37</v>
@@ -4522,11 +4533,11 @@
       </c>
       <c r="I22" s="74">
         <f>SUM(I20:I21)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="J22" s="75">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="K22" s="76"/>
       <c r="L22" s="77"/>
@@ -4662,7 +4673,7 @@
       </c>
       <c r="AU22" s="80">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AV22" s="80">
         <f t="shared" si="10"/>
@@ -4670,11 +4681,11 @@
       </c>
       <c r="AW22" s="91">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AX22" s="92">
         <f t="shared" si="10"/>
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="AY22" s="102"/>
       <c r="AZ22" s="103"/>
@@ -5057,11 +5068,11 @@
       </c>
       <c r="I26" s="43">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="J26" s="44">
         <f t="shared" si="12"/>
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="K26" s="45"/>
       <c r="M26" s="105"/>
@@ -5181,7 +5192,7 @@
       </c>
       <c r="AU26" s="43">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AV26" s="43">
         <f t="shared" si="13"/>
@@ -5189,11 +5200,11 @@
       </c>
       <c r="AW26" s="49">
         <f>AW9+AW13+AW19+AW22+AW25</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AX26" s="43">
         <f t="shared" si="13"/>
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="AY26" s="106"/>
       <c r="AZ26" s="107"/>
@@ -5298,10 +5309,10 @@
       <c r="AV28" s="43"/>
       <c r="AW28" s="49"/>
       <c r="AX28" s="50"/>
-      <c r="AY28" s="348" t="s">
+      <c r="AY28" s="355" t="s">
         <v>42</v>
       </c>
-      <c r="AZ28" s="349"/>
+      <c r="AZ28" s="356"/>
     </row>
     <row r="29" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A29" s="29"/>
@@ -6319,10 +6330,10 @@
       <c r="AV37" s="123"/>
       <c r="AW37" s="129"/>
       <c r="AX37" s="130"/>
-      <c r="AY37" s="350" t="s">
+      <c r="AY37" s="357" t="s">
         <v>47</v>
       </c>
-      <c r="AZ37" s="351"/>
+      <c r="AZ37" s="358"/>
     </row>
     <row r="38" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A38" s="29"/>
@@ -8553,11 +8564,11 @@
       </c>
       <c r="I57" s="135">
         <f>AW57</f>
-        <v>0</v>
+        <v>5.75</v>
       </c>
       <c r="J57" s="136">
         <f t="shared" si="27"/>
-        <v>28.25</v>
+        <v>34</v>
       </c>
       <c r="K57" s="137"/>
       <c r="L57" s="138"/>
@@ -8629,17 +8640,26 @@
       </c>
       <c r="AQ57" s="61"/>
       <c r="AR57" s="141"/>
-      <c r="AS57" s="135"/>
-      <c r="AT57" s="135"/>
-      <c r="AU57" s="135"/>
-      <c r="AV57" s="135"/>
+      <c r="AS57" s="135">
+        <f>1+1.25</f>
+        <v>2.25</v>
+      </c>
+      <c r="AT57" s="135">
+        <v>0.25</v>
+      </c>
+      <c r="AU57" s="135">
+        <v>2.25</v>
+      </c>
+      <c r="AV57" s="135">
+        <v>1</v>
+      </c>
       <c r="AW57" s="142">
         <f>SUM(AR57:AV57)</f>
-        <v>0</v>
+        <v>5.75</v>
       </c>
       <c r="AX57" s="65">
         <f>U57+AB57+AI57+AP57+AW57</f>
-        <v>28.25</v>
+        <v>34</v>
       </c>
       <c r="AY57" s="164"/>
       <c r="AZ57" s="165" t="s">
@@ -8769,148 +8789,148 @@
       </c>
       <c r="I59" s="166">
         <f>AW134</f>
-        <v>5</v>
+        <v>16.75</v>
       </c>
       <c r="J59" s="167">
         <f t="shared" si="27"/>
-        <v>41.75</v>
+        <v>53.5</v>
       </c>
       <c r="K59" s="137"/>
       <c r="L59" s="138"/>
-      <c r="M59" s="325" t="s">
+      <c r="M59" s="324" t="s">
         <v>30</v>
       </c>
-      <c r="N59" s="326" t="s">
+      <c r="N59" s="325" t="s">
         <v>110</v>
       </c>
       <c r="O59" s="61"/>
-      <c r="P59" s="327">
+      <c r="P59" s="326">
         <f>P134</f>
         <v>3</v>
       </c>
-      <c r="Q59" s="328">
+      <c r="Q59" s="327">
         <f t="shared" ref="Q59:T59" si="40">Q134</f>
         <v>0</v>
       </c>
-      <c r="R59" s="328">
+      <c r="R59" s="327">
         <f t="shared" si="40"/>
         <v>2</v>
       </c>
-      <c r="S59" s="328">
+      <c r="S59" s="327">
         <f t="shared" si="40"/>
         <v>0.5</v>
       </c>
-      <c r="T59" s="328">
+      <c r="T59" s="327">
         <f t="shared" si="40"/>
         <v>7</v>
       </c>
-      <c r="U59" s="329">
+      <c r="U59" s="328">
         <f>U134</f>
         <v>12.5</v>
       </c>
       <c r="V59" s="61"/>
-      <c r="W59" s="327">
+      <c r="W59" s="326">
         <f>W134</f>
         <v>4</v>
       </c>
-      <c r="X59" s="328">
+      <c r="X59" s="327">
         <f t="shared" ref="X59:AA59" si="41">X134</f>
         <v>8.25</v>
       </c>
-      <c r="Y59" s="328">
+      <c r="Y59" s="327">
         <f t="shared" si="41"/>
         <v>2.75</v>
       </c>
-      <c r="Z59" s="328">
+      <c r="Z59" s="327">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="AA59" s="328">
+      <c r="AA59" s="327">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="AB59" s="329">
+      <c r="AB59" s="328">
         <f>AB134</f>
         <v>15</v>
       </c>
       <c r="AC59" s="61"/>
-      <c r="AD59" s="327">
+      <c r="AD59" s="326">
         <f>AD134</f>
         <v>0</v>
       </c>
-      <c r="AE59" s="328">
+      <c r="AE59" s="327">
         <f t="shared" ref="AE59:AH59" si="42">AE134</f>
         <v>0</v>
       </c>
-      <c r="AF59" s="328">
+      <c r="AF59" s="327">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
-      <c r="AG59" s="328">
+      <c r="AG59" s="327">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
-      <c r="AH59" s="328">
+      <c r="AH59" s="327">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
-      <c r="AI59" s="329">
+      <c r="AI59" s="328">
         <f>AI134</f>
         <v>0</v>
       </c>
       <c r="AJ59" s="61"/>
-      <c r="AK59" s="327">
+      <c r="AK59" s="326">
         <f>AK134</f>
         <v>0</v>
       </c>
-      <c r="AL59" s="328">
+      <c r="AL59" s="327">
         <f t="shared" ref="AL59:AO59" si="43">AL134</f>
         <v>4</v>
       </c>
-      <c r="AM59" s="328">
+      <c r="AM59" s="327">
         <f t="shared" si="43"/>
         <v>1.25</v>
       </c>
-      <c r="AN59" s="328">
+      <c r="AN59" s="327">
         <f t="shared" si="43"/>
         <v>1.75</v>
       </c>
-      <c r="AO59" s="328">
+      <c r="AO59" s="327">
         <f t="shared" si="43"/>
         <v>2.25</v>
       </c>
-      <c r="AP59" s="329">
+      <c r="AP59" s="328">
         <f>AP134</f>
         <v>9.25</v>
       </c>
       <c r="AQ59" s="61"/>
-      <c r="AR59" s="327">
+      <c r="AR59" s="326">
         <f>AR134</f>
         <v>5</v>
       </c>
-      <c r="AS59" s="328">
+      <c r="AS59" s="327">
         <f t="shared" ref="AS59:AV59" si="44">AS134</f>
-        <v>0</v>
-      </c>
-      <c r="AT59" s="328">
+        <v>3.75</v>
+      </c>
+      <c r="AT59" s="327">
         <f t="shared" si="44"/>
-        <v>0</v>
-      </c>
-      <c r="AU59" s="328">
+        <v>3.5</v>
+      </c>
+      <c r="AU59" s="327">
         <f t="shared" si="44"/>
-        <v>0</v>
-      </c>
-      <c r="AV59" s="328">
+        <v>2.5</v>
+      </c>
+      <c r="AV59" s="327">
         <f t="shared" si="44"/>
-        <v>0</v>
-      </c>
-      <c r="AW59" s="329">
+        <v>2</v>
+      </c>
+      <c r="AW59" s="328">
         <f>AW134</f>
-        <v>5</v>
+        <v>16.75</v>
       </c>
       <c r="AX59" s="65">
         <f>U59+AB59+AI59+AP59+AW59</f>
-        <v>41.75</v>
+        <v>53.5</v>
       </c>
       <c r="AY59" s="143"/>
       <c r="AZ59" s="144" t="s">
@@ -8940,11 +8960,11 @@
       </c>
       <c r="I60" s="152">
         <f>SUM(I56:I59)</f>
-        <v>5</v>
+        <v>22.5</v>
       </c>
       <c r="J60" s="153">
         <f t="shared" si="27"/>
-        <v>70</v>
+        <v>87.5</v>
       </c>
       <c r="K60" s="154"/>
       <c r="L60" s="155"/>
@@ -9072,27 +9092,27 @@
       </c>
       <c r="AS60" s="80">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AT60" s="80">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="AU60" s="80">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>4.75</v>
       </c>
       <c r="AV60" s="168">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AW60" s="169">
         <f t="shared" si="45"/>
-        <v>5</v>
+        <v>22.5</v>
       </c>
       <c r="AX60" s="92">
         <f t="shared" si="45"/>
-        <v>70</v>
+        <v>87.5</v>
       </c>
       <c r="AY60" s="158"/>
       <c r="AZ60" s="159"/>
@@ -9119,11 +9139,11 @@
       </c>
       <c r="I61" s="171">
         <f t="shared" si="46"/>
-        <v>5</v>
+        <v>22.5</v>
       </c>
       <c r="J61" s="171">
         <f t="shared" si="46"/>
-        <v>70</v>
+        <v>87.5</v>
       </c>
       <c r="K61" s="125"/>
       <c r="M61" s="172"/>
@@ -9235,27 +9255,27 @@
       </c>
       <c r="AS61" s="123">
         <f t="shared" ref="AS61:AX61" si="51">AS42+AS50+AS55+AS46+AS60</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AT61" s="123">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="AU61" s="123">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>4.75</v>
       </c>
       <c r="AV61" s="171">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AW61" s="173">
         <f t="shared" si="51"/>
-        <v>5</v>
+        <v>22.5</v>
       </c>
       <c r="AX61" s="123">
         <f t="shared" si="51"/>
-        <v>70</v>
+        <v>87.5</v>
       </c>
       <c r="AY61" s="174"/>
       <c r="AZ61" s="175"/>
@@ -9360,10 +9380,10 @@
       <c r="AV63" s="123"/>
       <c r="AW63" s="129"/>
       <c r="AX63" s="130"/>
-      <c r="AY63" s="350" t="s">
+      <c r="AY63" s="357" t="s">
         <v>66</v>
       </c>
-      <c r="AZ63" s="351"/>
+      <c r="AZ63" s="358"/>
     </row>
     <row r="64" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A64" s="29"/>
@@ -9921,10 +9941,10 @@
       <c r="AV69" s="180"/>
       <c r="AW69" s="186"/>
       <c r="AX69" s="187"/>
-      <c r="AY69" s="336" t="s">
+      <c r="AY69" s="343" t="s">
         <v>69</v>
       </c>
-      <c r="AZ69" s="337"/>
+      <c r="AZ69" s="344"/>
     </row>
     <row r="70" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A70" s="29"/>
@@ -10380,10 +10400,10 @@
       <c r="AV74" s="180"/>
       <c r="AW74" s="186"/>
       <c r="AX74" s="187"/>
-      <c r="AY74" s="336" t="s">
+      <c r="AY74" s="343" t="s">
         <v>72</v>
       </c>
-      <c r="AZ74" s="337"/>
+      <c r="AZ74" s="344"/>
     </row>
     <row r="75" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A75" s="29"/>
@@ -10506,11 +10526,11 @@
       </c>
       <c r="I76" s="192">
         <f>AW76</f>
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="J76" s="193">
         <f>SUM(E76:I76)</f>
-        <v>1.5</v>
+        <v>2.75</v>
       </c>
       <c r="K76" s="194"/>
       <c r="L76" s="195"/>
@@ -10565,16 +10585,19 @@
         <v>0.75</v>
       </c>
       <c r="AS76" s="192"/>
-      <c r="AT76" s="192"/>
+      <c r="AT76" s="192">
+        <f>1.25</f>
+        <v>1.25</v>
+      </c>
       <c r="AU76" s="192"/>
       <c r="AV76" s="192"/>
       <c r="AW76" s="199">
         <f>SUM(AR76:AV76)</f>
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="AX76" s="65">
         <f>U76+AB76+AI76+AP76+AW76</f>
-        <v>1.5</v>
+        <v>2.75</v>
       </c>
       <c r="AY76" s="196" t="s">
         <v>74</v>
@@ -10719,11 +10742,11 @@
       </c>
       <c r="I78" s="192">
         <f>AW78</f>
-        <v>1.25</v>
+        <v>7.5</v>
       </c>
       <c r="J78" s="193">
         <f>SUM(E78:I78)</f>
-        <v>11.5</v>
+        <v>17.75</v>
       </c>
       <c r="K78" s="194"/>
       <c r="L78" s="195"/>
@@ -10771,7 +10794,7 @@
       <c r="AC78" s="61"/>
       <c r="AD78" s="198"/>
       <c r="AE78" s="192"/>
-      <c r="AF78" s="331"/>
+      <c r="AF78" s="330"/>
       <c r="AG78" s="192"/>
       <c r="AH78" s="192"/>
       <c r="AI78" s="199">
@@ -10800,17 +10823,26 @@
       <c r="AR78" s="198">
         <v>1.25</v>
       </c>
-      <c r="AS78" s="192"/>
-      <c r="AT78" s="192"/>
-      <c r="AU78" s="192"/>
-      <c r="AV78" s="192"/>
+      <c r="AS78" s="192">
+        <f>0.25+0.75+0.25</f>
+        <v>1.25</v>
+      </c>
+      <c r="AT78" s="192">
+        <v>0.75</v>
+      </c>
+      <c r="AU78" s="192">
+        <v>2.25</v>
+      </c>
+      <c r="AV78" s="192">
+        <v>2</v>
+      </c>
       <c r="AW78" s="199">
         <f>SUM(AR78:AV78)</f>
-        <v>1.25</v>
+        <v>7.5</v>
       </c>
       <c r="AX78" s="65">
         <f>U78+AB78+AI78+AP78+AW78</f>
-        <v>11.5</v>
+        <v>17.75</v>
       </c>
       <c r="AY78" s="196" t="s">
         <v>77</v>
@@ -10839,11 +10871,11 @@
       </c>
       <c r="I79" s="180">
         <f t="shared" si="64"/>
-        <v>2</v>
+        <v>9.5</v>
       </c>
       <c r="J79" s="181">
         <f t="shared" si="64"/>
-        <v>23.25</v>
+        <v>30.75</v>
       </c>
       <c r="K79" s="182"/>
       <c r="M79" s="202"/>
@@ -10955,27 +10987,27 @@
       </c>
       <c r="AS79" s="180">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="AT79" s="180">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AU79" s="180">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="AV79" s="180">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW79" s="186">
         <f t="shared" si="69"/>
-        <v>2</v>
+        <v>9.5</v>
       </c>
       <c r="AX79" s="187">
         <f t="shared" si="69"/>
-        <v>23.25</v>
+        <v>30.75</v>
       </c>
       <c r="AY79" s="203"/>
       <c r="AZ79" s="204"/>
@@ -11079,10 +11111,10 @@
       <c r="AV81" s="180"/>
       <c r="AW81" s="186"/>
       <c r="AX81" s="187"/>
-      <c r="AY81" s="336" t="s">
+      <c r="AY81" s="343" t="s">
         <v>78</v>
       </c>
-      <c r="AZ81" s="337"/>
+      <c r="AZ81" s="344"/>
     </row>
     <row r="82" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A82" s="29"/>
@@ -11205,11 +11237,11 @@
       </c>
       <c r="I83" s="192">
         <f>AW83</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J83" s="193">
         <f>SUM(E83:I83)</f>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="K83" s="194"/>
       <c r="L83" s="195" t="s">
@@ -11271,16 +11303,19 @@
         <v>1</v>
       </c>
       <c r="AS83" s="192"/>
-      <c r="AT83" s="192"/>
+      <c r="AT83" s="192">
+        <f>0.75+0.25</f>
+        <v>1</v>
+      </c>
       <c r="AU83" s="192"/>
       <c r="AV83" s="192"/>
       <c r="AW83" s="199">
         <f>SUM(AR83:AV83)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AX83" s="65">
         <f>U83+AB83+AI83+AP83+AW83</f>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="AY83" s="196" t="s">
         <v>80</v>
@@ -11309,11 +11344,11 @@
       </c>
       <c r="I84" s="180">
         <f t="shared" si="70"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J84" s="181">
         <f t="shared" si="70"/>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="K84" s="182"/>
       <c r="M84" s="202"/>
@@ -11429,7 +11464,7 @@
       </c>
       <c r="AT84" s="180">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU84" s="180">
         <f t="shared" si="75"/>
@@ -11441,11 +11476,11 @@
       </c>
       <c r="AW84" s="186">
         <f t="shared" si="75"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AX84" s="187">
         <f t="shared" si="75"/>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="AY84" s="203"/>
       <c r="AZ84" s="204"/>
@@ -11549,10 +11584,10 @@
       <c r="AV86" s="209"/>
       <c r="AW86" s="215"/>
       <c r="AX86" s="216"/>
-      <c r="AY86" s="341" t="s">
+      <c r="AY86" s="348" t="s">
         <v>81</v>
       </c>
-      <c r="AZ86" s="342"/>
+      <c r="AZ86" s="349"/>
     </row>
     <row r="87" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A87" s="29"/>
@@ -11677,11 +11712,11 @@
       </c>
       <c r="I88" s="221">
         <f>AW88</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J88" s="222">
         <f>SUM(E88:I88)</f>
-        <v>65.25</v>
+        <v>68.25</v>
       </c>
       <c r="K88" s="223"/>
       <c r="L88" s="224"/>
@@ -11752,14 +11787,16 @@
       <c r="AS88" s="221"/>
       <c r="AT88" s="221"/>
       <c r="AU88" s="221"/>
-      <c r="AV88" s="221"/>
+      <c r="AV88" s="221">
+        <v>3</v>
+      </c>
       <c r="AW88" s="228">
         <f>SUM(AR88:AV88)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AX88" s="65">
         <f>U88+AB88+AI88+AP88+AW88</f>
-        <v>65.25</v>
+        <v>68.25</v>
       </c>
       <c r="AY88" s="225" t="s">
         <v>83</v>
@@ -11788,11 +11825,11 @@
       </c>
       <c r="I89" s="209">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J89" s="210">
         <f t="shared" si="76"/>
-        <v>73.25</v>
+        <v>76.25</v>
       </c>
       <c r="K89" s="211"/>
       <c r="M89" s="231"/>
@@ -11916,15 +11953,15 @@
       </c>
       <c r="AV89" s="209">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AW89" s="215">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AX89" s="216">
         <f t="shared" si="81"/>
-        <v>73.25</v>
+        <v>76.25</v>
       </c>
       <c r="AY89" s="232"/>
       <c r="AZ89" s="233"/>
@@ -12000,60 +12037,60 @@
       </c>
       <c r="I91" s="234">
         <f t="shared" si="82"/>
-        <v>5</v>
+        <v>22.75</v>
       </c>
       <c r="J91" s="236">
         <f t="shared" si="82"/>
-        <v>74.5</v>
+        <v>92.25</v>
       </c>
       <c r="K91" s="234"/>
       <c r="L91" s="234"/>
       <c r="M91" s="237"/>
       <c r="N91" s="238"/>
       <c r="O91" s="37"/>
-      <c r="P91" s="343" t="s">
+      <c r="P91" s="350" t="s">
         <v>8</v>
       </c>
-      <c r="Q91" s="344"/>
-      <c r="R91" s="344"/>
-      <c r="S91" s="344"/>
-      <c r="T91" s="345"/>
+      <c r="Q91" s="351"/>
+      <c r="R91" s="351"/>
+      <c r="S91" s="351"/>
+      <c r="T91" s="352"/>
       <c r="U91" s="239"/>
       <c r="V91" s="240"/>
-      <c r="W91" s="343" t="s">
+      <c r="W91" s="350" t="s">
         <v>10</v>
       </c>
-      <c r="X91" s="344"/>
-      <c r="Y91" s="344"/>
-      <c r="Z91" s="344"/>
-      <c r="AA91" s="345"/>
+      <c r="X91" s="351"/>
+      <c r="Y91" s="351"/>
+      <c r="Z91" s="351"/>
+      <c r="AA91" s="352"/>
       <c r="AB91" s="239"/>
       <c r="AC91" s="240"/>
-      <c r="AD91" s="343" t="s">
+      <c r="AD91" s="350" t="s">
         <v>11</v>
       </c>
-      <c r="AE91" s="344"/>
-      <c r="AF91" s="344"/>
-      <c r="AG91" s="344"/>
-      <c r="AH91" s="345"/>
+      <c r="AE91" s="351"/>
+      <c r="AF91" s="351"/>
+      <c r="AG91" s="351"/>
+      <c r="AH91" s="352"/>
       <c r="AI91" s="239"/>
       <c r="AJ91" s="240"/>
-      <c r="AK91" s="343" t="s">
+      <c r="AK91" s="350" t="s">
         <v>12</v>
       </c>
-      <c r="AL91" s="344"/>
-      <c r="AM91" s="344"/>
-      <c r="AN91" s="344"/>
-      <c r="AO91" s="345"/>
+      <c r="AL91" s="351"/>
+      <c r="AM91" s="351"/>
+      <c r="AN91" s="351"/>
+      <c r="AO91" s="352"/>
       <c r="AP91" s="239"/>
       <c r="AQ91" s="240"/>
-      <c r="AR91" s="343" t="s">
+      <c r="AR91" s="350" t="s">
         <v>13</v>
       </c>
-      <c r="AS91" s="344"/>
-      <c r="AT91" s="344"/>
-      <c r="AU91" s="344"/>
-      <c r="AV91" s="345"/>
+      <c r="AS91" s="351"/>
+      <c r="AT91" s="351"/>
+      <c r="AU91" s="351"/>
+      <c r="AV91" s="352"/>
       <c r="AW91" s="112"/>
       <c r="AX91" s="241"/>
       <c r="AY91" s="237"/>
@@ -12084,50 +12121,50 @@
       </c>
       <c r="I92" s="234">
         <f t="shared" si="83"/>
-        <v>3</v>
+        <v>14.5</v>
       </c>
       <c r="J92" s="236">
         <f t="shared" si="83"/>
-        <v>100</v>
+        <v>111.5</v>
       </c>
       <c r="K92" s="234"/>
       <c r="L92" s="234"/>
       <c r="M92" s="237"/>
       <c r="N92" s="238"/>
       <c r="O92" s="37"/>
-      <c r="P92" s="343"/>
-      <c r="Q92" s="344"/>
-      <c r="R92" s="344"/>
-      <c r="S92" s="344"/>
-      <c r="T92" s="345"/>
+      <c r="P92" s="350"/>
+      <c r="Q92" s="351"/>
+      <c r="R92" s="351"/>
+      <c r="S92" s="351"/>
+      <c r="T92" s="352"/>
       <c r="U92" s="239"/>
       <c r="V92" s="240"/>
-      <c r="W92" s="343"/>
-      <c r="X92" s="344"/>
-      <c r="Y92" s="344"/>
-      <c r="Z92" s="344"/>
-      <c r="AA92" s="345"/>
+      <c r="W92" s="350"/>
+      <c r="X92" s="351"/>
+      <c r="Y92" s="351"/>
+      <c r="Z92" s="351"/>
+      <c r="AA92" s="352"/>
       <c r="AB92" s="239"/>
       <c r="AC92" s="240"/>
-      <c r="AD92" s="343"/>
-      <c r="AE92" s="344"/>
-      <c r="AF92" s="344"/>
-      <c r="AG92" s="344"/>
-      <c r="AH92" s="345"/>
+      <c r="AD92" s="350"/>
+      <c r="AE92" s="351"/>
+      <c r="AF92" s="351"/>
+      <c r="AG92" s="351"/>
+      <c r="AH92" s="352"/>
       <c r="AI92" s="239"/>
       <c r="AJ92" s="240"/>
-      <c r="AK92" s="343"/>
-      <c r="AL92" s="344"/>
-      <c r="AM92" s="344"/>
-      <c r="AN92" s="344"/>
-      <c r="AO92" s="345"/>
+      <c r="AK92" s="350"/>
+      <c r="AL92" s="351"/>
+      <c r="AM92" s="351"/>
+      <c r="AN92" s="351"/>
+      <c r="AO92" s="352"/>
       <c r="AP92" s="239"/>
       <c r="AQ92" s="240"/>
-      <c r="AR92" s="343"/>
-      <c r="AS92" s="344"/>
-      <c r="AT92" s="344"/>
-      <c r="AU92" s="344"/>
-      <c r="AV92" s="345"/>
+      <c r="AR92" s="350"/>
+      <c r="AS92" s="351"/>
+      <c r="AT92" s="351"/>
+      <c r="AU92" s="351"/>
+      <c r="AV92" s="352"/>
       <c r="AW92" s="112"/>
       <c r="AX92" s="241"/>
       <c r="AY92" s="237"/>
@@ -12158,11 +12195,11 @@
       </c>
       <c r="I93" s="242">
         <f t="shared" si="84"/>
-        <v>8</v>
+        <v>37.25</v>
       </c>
       <c r="J93" s="244">
         <f t="shared" si="84"/>
-        <v>174.5</v>
+        <v>203.75</v>
       </c>
       <c r="K93" s="242"/>
       <c r="L93" s="242"/>
@@ -12171,113 +12208,113 @@
       </c>
       <c r="N93" s="246"/>
       <c r="O93" s="247"/>
-      <c r="P93" s="330">
+      <c r="P93" s="329">
         <f>P26+P89+P84+P79+P72+P67+P61+P35</f>
         <v>7.75</v>
       </c>
-      <c r="Q93" s="330">
+      <c r="Q93" s="329">
         <f t="shared" ref="Q93:T93" si="85">Q26+Q89+Q84+Q79+Q72+Q67+Q61+Q35</f>
         <v>8</v>
       </c>
-      <c r="R93" s="330">
+      <c r="R93" s="329">
         <f t="shared" si="85"/>
         <v>7.5</v>
       </c>
-      <c r="S93" s="330">
+      <c r="S93" s="329">
         <f t="shared" si="85"/>
         <v>8</v>
       </c>
-      <c r="T93" s="330">
+      <c r="T93" s="329">
         <f t="shared" si="85"/>
         <v>12.5</v>
       </c>
       <c r="U93" s="246"/>
       <c r="V93" s="246"/>
-      <c r="W93" s="330">
+      <c r="W93" s="329">
         <f>W26+W89+W84+W79+W72+W67+W61+W35</f>
         <v>8.25</v>
       </c>
-      <c r="X93" s="330">
+      <c r="X93" s="329">
         <f t="shared" ref="X93:AA93" si="86">X26+X89+X84+X79+X72+X67+X61+X35</f>
         <v>11</v>
       </c>
-      <c r="Y93" s="330">
+      <c r="Y93" s="329">
         <f t="shared" si="86"/>
         <v>8</v>
       </c>
-      <c r="Z93" s="330">
+      <c r="Z93" s="329">
         <f t="shared" si="86"/>
         <v>8</v>
       </c>
-      <c r="AA93" s="330">
+      <c r="AA93" s="329">
         <f t="shared" si="86"/>
         <v>8</v>
       </c>
       <c r="AB93" s="246"/>
       <c r="AC93" s="246"/>
-      <c r="AD93" s="330">
+      <c r="AD93" s="329">
         <f>AD26+AD89+AD84+AD79+AD72+AD67+AD61+AD35</f>
         <v>8</v>
       </c>
-      <c r="AE93" s="330">
+      <c r="AE93" s="329">
         <f t="shared" ref="AE93:AH93" si="87">AE26+AE89+AE84+AE79+AE72+AE67+AE61+AE35</f>
         <v>8</v>
       </c>
-      <c r="AF93" s="330">
+      <c r="AF93" s="329">
         <f t="shared" si="87"/>
         <v>8</v>
       </c>
-      <c r="AG93" s="330">
+      <c r="AG93" s="329">
         <f t="shared" si="87"/>
         <v>8</v>
       </c>
-      <c r="AH93" s="330">
+      <c r="AH93" s="329">
         <f t="shared" si="87"/>
         <v>8</v>
       </c>
       <c r="AI93" s="246"/>
       <c r="AJ93" s="246"/>
-      <c r="AK93" s="330">
+      <c r="AK93" s="329">
         <f>AK26+AK89+AK84+AK79+AK72+AK67+AK61+AK35</f>
         <v>8</v>
       </c>
-      <c r="AL93" s="330">
+      <c r="AL93" s="329">
         <f t="shared" ref="AL93:AO93" si="88">AL26+AL89+AL84+AL79+AL72+AL67+AL61+AL35</f>
         <v>9</v>
       </c>
-      <c r="AM93" s="330">
+      <c r="AM93" s="329">
         <f t="shared" si="88"/>
         <v>8.25</v>
       </c>
-      <c r="AN93" s="330">
+      <c r="AN93" s="329">
         <f t="shared" si="88"/>
         <v>6.5</v>
       </c>
-      <c r="AO93" s="330">
+      <c r="AO93" s="329">
         <f t="shared" si="88"/>
         <v>7.75</v>
       </c>
       <c r="AP93" s="246"/>
       <c r="AQ93" s="246"/>
-      <c r="AR93" s="330">
+      <c r="AR93" s="329">
         <f>AR26+AR89+AR84+AR79+AR72+AR67+AR61+AR35</f>
         <v>8</v>
       </c>
-      <c r="AS93" s="330">
+      <c r="AS93" s="329">
         <f t="shared" ref="AS93:AV93" si="89">AS26+AS89+AS84+AS79+AS72+AS67+AS61+AS35</f>
-        <v>0</v>
-      </c>
-      <c r="AT93" s="330">
+        <v>7.25</v>
+      </c>
+      <c r="AT93" s="329">
         <f t="shared" si="89"/>
-        <v>0</v>
-      </c>
-      <c r="AU93" s="330">
+        <v>6.75</v>
+      </c>
+      <c r="AU93" s="329">
         <f t="shared" si="89"/>
-        <v>0</v>
-      </c>
-      <c r="AV93" s="330">
+        <v>7.25</v>
+      </c>
+      <c r="AV93" s="329">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AW93" s="246"/>
       <c r="AX93" s="246"/>
@@ -12309,14 +12346,14 @@
       </c>
       <c r="I94" s="234">
         <f>40-I93</f>
-        <v>32</v>
+        <v>2.75</v>
       </c>
       <c r="J94" s="236">
         <f>SUM(E94:I94)</f>
-        <v>25.5</v>
+        <v>-3.75</v>
       </c>
       <c r="K94" s="234"/>
-      <c r="L94" s="334" t="s">
+      <c r="L94" s="333" t="s">
         <v>121</v>
       </c>
       <c r="M94" s="110" t="s">
@@ -12324,113 +12361,113 @@
       </c>
       <c r="N94" s="111"/>
       <c r="O94" s="37"/>
-      <c r="P94" s="332">
+      <c r="P94" s="331">
         <f>8-P93</f>
         <v>0.25</v>
       </c>
-      <c r="Q94" s="320">
+      <c r="Q94" s="319">
         <f t="shared" ref="Q94:T94" si="90">8-Q93</f>
         <v>0</v>
       </c>
-      <c r="R94" s="320">
+      <c r="R94" s="319">
         <f t="shared" si="90"/>
         <v>0.5</v>
       </c>
-      <c r="S94" s="320">
+      <c r="S94" s="319">
         <f t="shared" si="90"/>
         <v>0</v>
       </c>
-      <c r="T94" s="333">
+      <c r="T94" s="332">
         <f t="shared" si="90"/>
         <v>-4.5</v>
       </c>
       <c r="U94" s="111"/>
       <c r="V94" s="37"/>
-      <c r="W94" s="332">
+      <c r="W94" s="331">
         <f>8-W93</f>
         <v>-0.25</v>
       </c>
-      <c r="X94" s="320">
+      <c r="X94" s="319">
         <f t="shared" ref="X94" si="91">8-X93</f>
         <v>-3</v>
       </c>
-      <c r="Y94" s="320">
+      <c r="Y94" s="319">
         <f t="shared" ref="Y94" si="92">8-Y93</f>
         <v>0</v>
       </c>
-      <c r="Z94" s="320">
+      <c r="Z94" s="319">
         <f t="shared" ref="Z94" si="93">8-Z93</f>
         <v>0</v>
       </c>
-      <c r="AA94" s="333">
+      <c r="AA94" s="332">
         <f t="shared" ref="AA94" si="94">8-AA93</f>
         <v>0</v>
       </c>
       <c r="AB94" s="112"/>
       <c r="AC94" s="37"/>
-      <c r="AD94" s="332">
+      <c r="AD94" s="331">
         <f>8-AD93</f>
         <v>0</v>
       </c>
-      <c r="AE94" s="320">
+      <c r="AE94" s="319">
         <f t="shared" ref="AE94" si="95">8-AE93</f>
         <v>0</v>
       </c>
-      <c r="AF94" s="320">
+      <c r="AF94" s="319">
         <f t="shared" ref="AF94" si="96">8-AF93</f>
         <v>0</v>
       </c>
-      <c r="AG94" s="320">
+      <c r="AG94" s="319">
         <f t="shared" ref="AG94" si="97">8-AG93</f>
         <v>0</v>
       </c>
-      <c r="AH94" s="333">
+      <c r="AH94" s="332">
         <f t="shared" ref="AH94" si="98">8-AH93</f>
         <v>0</v>
       </c>
       <c r="AI94" s="112"/>
       <c r="AJ94" s="37"/>
-      <c r="AK94" s="332">
+      <c r="AK94" s="331">
         <f>8-AK93</f>
         <v>0</v>
       </c>
-      <c r="AL94" s="320">
+      <c r="AL94" s="319">
         <f t="shared" ref="AL94" si="99">8-AL93</f>
         <v>-1</v>
       </c>
-      <c r="AM94" s="320">
+      <c r="AM94" s="319">
         <f t="shared" ref="AM94" si="100">8-AM93</f>
         <v>-0.25</v>
       </c>
-      <c r="AN94" s="320">
+      <c r="AN94" s="319">
         <f t="shared" ref="AN94" si="101">8-AN93</f>
         <v>1.5</v>
       </c>
-      <c r="AO94" s="333">
+      <c r="AO94" s="332">
         <f t="shared" ref="AO94" si="102">8-AO93</f>
         <v>0.25</v>
       </c>
       <c r="AP94" s="112"/>
       <c r="AQ94" s="37"/>
-      <c r="AR94" s="332">
+      <c r="AR94" s="331">
         <f>8-AR93</f>
         <v>0</v>
       </c>
-      <c r="AS94" s="320">
+      <c r="AS94" s="319">
         <f t="shared" ref="AS94" si="103">8-AS93</f>
-        <v>8</v>
-      </c>
-      <c r="AT94" s="320">
+        <v>0.75</v>
+      </c>
+      <c r="AT94" s="319">
         <f t="shared" ref="AT94" si="104">8-AT93</f>
-        <v>8</v>
-      </c>
-      <c r="AU94" s="320">
+        <v>1.25</v>
+      </c>
+      <c r="AU94" s="319">
         <f t="shared" ref="AU94" si="105">8-AU93</f>
-        <v>8</v>
-      </c>
-      <c r="AV94" s="333">
+        <v>0.75</v>
+      </c>
+      <c r="AV94" s="332">
         <f t="shared" ref="AV94" si="106">8-AV93</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AW94" s="112"/>
       <c r="AX94" s="111"/>
@@ -12461,11 +12498,11 @@
       </c>
       <c r="I95" s="252">
         <f>I91/(40-I87-I88)*100</f>
-        <v>12.5</v>
+        <v>61.486486486486491</v>
       </c>
       <c r="J95" s="251">
         <f>AVERAGEIF(E95:I95,"&lt;&gt;0")</f>
-        <v>64.507113821138205</v>
+        <v>76.753735442759833</v>
       </c>
       <c r="K95" s="243" t="s">
         <v>89</v>
@@ -12475,9 +12512,9 @@
       <c r="N95" s="111"/>
       <c r="O95" s="37"/>
       <c r="P95" s="237"/>
-      <c r="Q95" s="317"/>
+      <c r="Q95" s="316"/>
       <c r="R95" s="37"/>
-      <c r="T95" s="320">
+      <c r="T95" s="319">
         <f>SUM(P93:T93)</f>
         <v>43.75</v>
       </c>
@@ -12486,7 +12523,7 @@
       <c r="W95" s="110"/>
       <c r="X95" s="37"/>
       <c r="Y95" s="37"/>
-      <c r="AA95" s="320">
+      <c r="AA95" s="319">
         <f>SUM(W93:AA93)</f>
         <v>43.25</v>
       </c>
@@ -12495,7 +12532,7 @@
       <c r="AD95" s="110"/>
       <c r="AE95" s="37"/>
       <c r="AF95" s="37"/>
-      <c r="AH95" s="320">
+      <c r="AH95" s="319">
         <f>SUM(AD93:AH93)</f>
         <v>40</v>
       </c>
@@ -12504,7 +12541,7 @@
       <c r="AK95" s="110"/>
       <c r="AL95" s="37"/>
       <c r="AM95" s="37"/>
-      <c r="AO95" s="320">
+      <c r="AO95" s="319">
         <f>SUM(AK93:AO93)</f>
         <v>39.5</v>
       </c>
@@ -12513,9 +12550,9 @@
       <c r="AR95" s="110"/>
       <c r="AS95" s="37"/>
       <c r="AT95" s="37"/>
-      <c r="AV95" s="320">
+      <c r="AV95" s="319">
         <f>SUM(AR93:AV93)</f>
-        <v>8</v>
+        <v>37.25</v>
       </c>
       <c r="AW95" s="112"/>
       <c r="AX95" s="111"/>
@@ -12547,11 +12584,11 @@
       </c>
       <c r="I96" s="256">
         <f>I91/40*100</f>
-        <v>12.5</v>
+        <v>56.875</v>
       </c>
       <c r="J96" s="255">
         <f>AVERAGEIF(E96:I96,"&lt;&gt;0")</f>
-        <v>46.5625</v>
+        <v>57.65625</v>
       </c>
       <c r="K96" s="257" t="s">
         <v>89</v>
@@ -12654,10 +12691,10 @@
       <c r="AV101" s="267"/>
       <c r="AW101" s="269"/>
       <c r="AX101" s="267"/>
-      <c r="AY101" s="339" t="s">
+      <c r="AY101" s="346" t="s">
         <v>47</v>
       </c>
-      <c r="AZ101" s="340"/>
+      <c r="AZ101" s="347"/>
     </row>
     <row r="102" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A102" s="270"/>
@@ -12686,11 +12723,11 @@
       </c>
       <c r="I102" s="135">
         <f>AW102</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="J102" s="136">
-        <f t="shared" ref="J102:J106" si="107">SUM(E102:I102)</f>
-        <v>0.75</v>
+        <f t="shared" ref="J102:J134" si="107">SUM(E102:I102)</f>
+        <v>1</v>
       </c>
       <c r="K102" s="274"/>
       <c r="L102" s="275" t="s">
@@ -12702,7 +12739,7 @@
       <c r="N102" s="140" t="s">
         <v>109</v>
       </c>
-      <c r="O102" s="321"/>
+      <c r="O102" s="320"/>
       <c r="P102" s="141"/>
       <c r="Q102" s="135"/>
       <c r="R102" s="135"/>
@@ -12752,15 +12789,17 @@
       <c r="AR102" s="141"/>
       <c r="AS102" s="135"/>
       <c r="AT102" s="135"/>
-      <c r="AU102" s="135"/>
+      <c r="AU102" s="135">
+        <v>0.25</v>
+      </c>
       <c r="AV102" s="135"/>
       <c r="AW102" s="276">
         <f>SUM(AR102:AV102)</f>
-        <v>0</v>
-      </c>
-      <c r="AX102" s="323">
+        <v>0.25</v>
+      </c>
+      <c r="AX102" s="322">
         <f t="shared" ref="AX102:AX106" si="108">U102+AB102+AI102+AP102+AW102</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AY102" s="139" t="s">
         <v>108</v>
@@ -12792,17 +12831,17 @@
       </c>
       <c r="I103" s="152">
         <f>SUM(I98:I102)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="J103" s="153">
         <f t="shared" si="107"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="K103" s="280"/>
       <c r="L103" s="281"/>
       <c r="M103" s="156"/>
       <c r="N103" s="157"/>
-      <c r="O103" s="322">
+      <c r="O103" s="321">
         <f>SUM(O102)</f>
         <v>0</v>
       </c>
@@ -12932,7 +12971,7 @@
       </c>
       <c r="AU103" s="80">
         <f t="shared" ref="AU103" si="124">SUM(AU102)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AV103" s="168">
         <f t="shared" ref="AV103" si="125">SUM(AV102)</f>
@@ -12940,11 +12979,11 @@
       </c>
       <c r="AW103" s="282">
         <f>SUM(AW102)</f>
-        <v>0</v>
-      </c>
-      <c r="AX103" s="324">
+        <v>0.25</v>
+      </c>
+      <c r="AX103" s="323">
         <f>SUM(AX102)</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AY103" s="156"/>
       <c r="AZ103" s="157"/>
@@ -13040,7 +13079,7 @@
         <f>SUM(AR104:AV104)</f>
         <v>0</v>
       </c>
-      <c r="AX104" s="323">
+      <c r="AX104" s="322">
         <f t="shared" si="108"/>
         <v>0</v>
       </c>
@@ -13138,7 +13177,7 @@
         <f>SUM(AR105:AV105)</f>
         <v>0</v>
       </c>
-      <c r="AX105" s="323">
+      <c r="AX105" s="322">
         <f t="shared" si="108"/>
         <v>0</v>
       </c>
@@ -13234,7 +13273,7 @@
         <f>SUM(AR106:AV106)</f>
         <v>0</v>
       </c>
-      <c r="AX106" s="323">
+      <c r="AX106" s="322">
         <f t="shared" si="108"/>
         <v>0</v>
       </c>
@@ -13269,7 +13308,7 @@
         <v>0</v>
       </c>
       <c r="J107" s="153">
-        <f t="shared" si="126"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="K107" s="280"/>
@@ -13416,7 +13455,7 @@
         <f>SUM(AW104:AW106)</f>
         <v>0</v>
       </c>
-      <c r="AX107" s="324">
+      <c r="AX107" s="323">
         <f t="shared" ref="AX107" si="144">SUM(AX104:AX106)</f>
         <v>0</v>
       </c>
@@ -13452,15 +13491,16 @@
         <f>AW108</f>
         <v>0</v>
       </c>
-      <c r="J108" s="287">
-        <v>0</v>
-      </c>
-      <c r="K108" s="288"/>
-      <c r="L108" s="289"/>
-      <c r="M108" s="290" t="s">
+      <c r="J108" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K108" s="287"/>
+      <c r="L108" s="288"/>
+      <c r="M108" s="289" t="s">
         <v>95</v>
       </c>
-      <c r="N108" s="291" t="s">
+      <c r="N108" s="290" t="s">
         <v>61</v>
       </c>
       <c r="O108" s="61"/>
@@ -13513,14 +13553,14 @@
         <f>SUM(AR108:AV108)</f>
         <v>0</v>
       </c>
-      <c r="AX108" s="323">
+      <c r="AX108" s="322">
         <f>U108+AB108+AI108+AP108+AW108</f>
         <v>0</v>
       </c>
-      <c r="AY108" s="290" t="s">
+      <c r="AY108" s="289" t="s">
         <v>95</v>
       </c>
-      <c r="AZ108" s="291" t="s">
+      <c r="AZ108" s="290" t="s">
         <v>61</v>
       </c>
     </row>
@@ -13551,13 +13591,14 @@
         <f>AW109</f>
         <v>0</v>
       </c>
-      <c r="J109" s="287">
-        <v>0</v>
-      </c>
-      <c r="K109" s="288"/>
-      <c r="L109" s="289"/>
-      <c r="M109" s="290"/>
-      <c r="N109" s="291" t="s">
+      <c r="J109" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K109" s="287"/>
+      <c r="L109" s="288"/>
+      <c r="M109" s="289"/>
+      <c r="N109" s="290" t="s">
         <v>30</v>
       </c>
       <c r="O109" s="61"/>
@@ -13610,19 +13651,19 @@
         <f>SUM(AR109:AV109)</f>
         <v>0</v>
       </c>
-      <c r="AX109" s="323">
+      <c r="AX109" s="322">
         <f>U109+AB109+AI109+AP109+AW109</f>
         <v>0</v>
       </c>
-      <c r="AY109" s="290"/>
-      <c r="AZ109" s="291" t="s">
+      <c r="AY109" s="289"/>
+      <c r="AZ109" s="290" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="110" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A110" s="283"/>
       <c r="B110" s="284"/>
-      <c r="C110" s="292"/>
+      <c r="C110" s="291"/>
       <c r="D110" s="286" t="s">
         <v>30</v>
       </c>
@@ -13646,13 +13687,14 @@
         <f>AW110</f>
         <v>0</v>
       </c>
-      <c r="J110" s="287">
-        <v>0</v>
-      </c>
-      <c r="K110" s="288"/>
-      <c r="L110" s="289"/>
-      <c r="M110" s="293"/>
-      <c r="N110" s="291" t="s">
+      <c r="J110" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K110" s="287"/>
+      <c r="L110" s="288"/>
+      <c r="M110" s="292"/>
+      <c r="N110" s="290" t="s">
         <v>30</v>
       </c>
       <c r="O110" s="61"/>
@@ -13705,12 +13747,12 @@
         <f>SUM(AR110:AV110)</f>
         <v>0</v>
       </c>
-      <c r="AX110" s="323">
+      <c r="AX110" s="322">
         <f>U110+AB110+AI110+AP110+AW110</f>
         <v>0</v>
       </c>
-      <c r="AY110" s="293"/>
-      <c r="AZ110" s="291" t="s">
+      <c r="AY110" s="292"/>
+      <c r="AZ110" s="290" t="s">
         <v>30</v>
       </c>
     </row>
@@ -13740,7 +13782,7 @@
         <v>0</v>
       </c>
       <c r="J111" s="153">
-        <f>SUM(E111:I111)</f>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="K111" s="280"/>
@@ -13887,7 +13929,7 @@
         <f t="shared" si="146"/>
         <v>0</v>
       </c>
-      <c r="AX111" s="324">
+      <c r="AX111" s="323">
         <f t="shared" si="146"/>
         <v>0</v>
       </c>
@@ -13923,15 +13965,16 @@
         <f>AW112</f>
         <v>0</v>
       </c>
-      <c r="J112" s="287">
-        <v>0</v>
-      </c>
-      <c r="K112" s="288"/>
-      <c r="L112" s="289"/>
-      <c r="M112" s="290" t="s">
+      <c r="J112" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K112" s="287"/>
+      <c r="L112" s="288"/>
+      <c r="M112" s="289" t="s">
         <v>48</v>
       </c>
-      <c r="N112" s="291" t="s">
+      <c r="N112" s="290" t="s">
         <v>50</v>
       </c>
       <c r="O112" s="61"/>
@@ -13988,10 +14031,10 @@
         <f>U112+AB112+AI112+AP112+AW112</f>
         <v>0</v>
       </c>
-      <c r="AY112" s="290" t="s">
+      <c r="AY112" s="289" t="s">
         <v>48</v>
       </c>
-      <c r="AZ112" s="291" t="s">
+      <c r="AZ112" s="290" t="s">
         <v>50</v>
       </c>
     </row>
@@ -14022,13 +14065,14 @@
         <f>AW113</f>
         <v>0</v>
       </c>
-      <c r="J113" s="287">
-        <v>0</v>
-      </c>
-      <c r="K113" s="288"/>
-      <c r="L113" s="289"/>
-      <c r="M113" s="290"/>
-      <c r="N113" s="291" t="s">
+      <c r="J113" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K113" s="287"/>
+      <c r="L113" s="288"/>
+      <c r="M113" s="289"/>
+      <c r="N113" s="290" t="s">
         <v>49</v>
       </c>
       <c r="O113" s="61"/>
@@ -14085,15 +14129,15 @@
         <f>U113+AB113+AI113+AP113+AW113</f>
         <v>0</v>
       </c>
-      <c r="AY113" s="290"/>
-      <c r="AZ113" s="291" t="s">
+      <c r="AY113" s="289"/>
+      <c r="AZ113" s="290" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="114" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A114" s="283"/>
       <c r="B114" s="284"/>
-      <c r="C114" s="292"/>
+      <c r="C114" s="291"/>
       <c r="D114" s="286" t="s">
         <v>30</v>
       </c>
@@ -14117,13 +14161,14 @@
         <f>AW114</f>
         <v>0</v>
       </c>
-      <c r="J114" s="287">
-        <v>0</v>
-      </c>
-      <c r="K114" s="288"/>
-      <c r="L114" s="289"/>
-      <c r="M114" s="293"/>
-      <c r="N114" s="291" t="s">
+      <c r="J114" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K114" s="287"/>
+      <c r="L114" s="288"/>
+      <c r="M114" s="292"/>
+      <c r="N114" s="290" t="s">
         <v>30</v>
       </c>
       <c r="O114" s="61"/>
@@ -14180,16 +14225,16 @@
         <f>U114+AB114+AI114+AP114+AW114</f>
         <v>0</v>
       </c>
-      <c r="AY114" s="293"/>
-      <c r="AZ114" s="291" t="s">
+      <c r="AY114" s="292"/>
+      <c r="AZ114" s="290" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="115" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A115" s="283"/>
       <c r="B115" s="284"/>
-      <c r="C115" s="294"/>
-      <c r="D115" s="295"/>
+      <c r="C115" s="293"/>
+      <c r="D115" s="294"/>
       <c r="E115" s="150">
         <f>SUM(E112:E114)</f>
         <v>0</v>
@@ -14211,13 +14256,13 @@
         <v>0</v>
       </c>
       <c r="J115" s="153">
-        <f>SUM(E115:I115)</f>
-        <v>0</v>
-      </c>
-      <c r="K115" s="296"/>
-      <c r="L115" s="297"/>
-      <c r="M115" s="298"/>
-      <c r="N115" s="299"/>
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K115" s="295"/>
+      <c r="L115" s="296"/>
+      <c r="M115" s="297"/>
+      <c r="N115" s="298"/>
       <c r="O115" s="80">
         <f t="shared" ref="O115" si="147">SUM(O112:O114)</f>
         <v>0</v>
@@ -14362,8 +14407,8 @@
         <f t="shared" si="148"/>
         <v>0</v>
       </c>
-      <c r="AY115" s="298"/>
-      <c r="AZ115" s="299"/>
+      <c r="AY115" s="297"/>
+      <c r="AZ115" s="298"/>
     </row>
     <row r="116" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A116" s="283"/>
@@ -14394,15 +14439,16 @@
         <f>AW116</f>
         <v>0</v>
       </c>
-      <c r="J116" s="287">
-        <v>0</v>
-      </c>
-      <c r="K116" s="288"/>
-      <c r="L116" s="289"/>
-      <c r="M116" s="290" t="s">
+      <c r="J116" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K116" s="287"/>
+      <c r="L116" s="288"/>
+      <c r="M116" s="289" t="s">
         <v>52</v>
       </c>
-      <c r="N116" s="291" t="s">
+      <c r="N116" s="290" t="s">
         <v>96</v>
       </c>
       <c r="O116" s="61"/>
@@ -14459,10 +14505,10 @@
         <f>U116+AB116+AI116+AP116+AW116</f>
         <v>0</v>
       </c>
-      <c r="AY116" s="290" t="s">
+      <c r="AY116" s="289" t="s">
         <v>52</v>
       </c>
-      <c r="AZ116" s="291" t="s">
+      <c r="AZ116" s="290" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14493,13 +14539,14 @@
         <f>AW117</f>
         <v>0</v>
       </c>
-      <c r="J117" s="287">
-        <v>0</v>
-      </c>
-      <c r="K117" s="288"/>
-      <c r="L117" s="289"/>
-      <c r="M117" s="290"/>
-      <c r="N117" s="291" t="s">
+      <c r="J117" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K117" s="287"/>
+      <c r="L117" s="288"/>
+      <c r="M117" s="289"/>
+      <c r="N117" s="290" t="s">
         <v>97</v>
       </c>
       <c r="O117" s="61"/>
@@ -14556,15 +14603,15 @@
         <f>U117+AB117+AI117+AP117+AW117</f>
         <v>0</v>
       </c>
-      <c r="AY117" s="290"/>
-      <c r="AZ117" s="291" t="s">
+      <c r="AY117" s="289"/>
+      <c r="AZ117" s="290" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="118" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A118" s="283"/>
       <c r="B118" s="284"/>
-      <c r="C118" s="292"/>
+      <c r="C118" s="291"/>
       <c r="D118" s="286" t="s">
         <v>116</v>
       </c>
@@ -14588,13 +14635,14 @@
         <f>AW118</f>
         <v>0</v>
       </c>
-      <c r="J118" s="287">
-        <v>0</v>
-      </c>
-      <c r="K118" s="288"/>
-      <c r="L118" s="289"/>
-      <c r="M118" s="293"/>
-      <c r="N118" s="291" t="s">
+      <c r="J118" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K118" s="287"/>
+      <c r="L118" s="288"/>
+      <c r="M118" s="292"/>
+      <c r="N118" s="290" t="s">
         <v>116</v>
       </c>
       <c r="O118" s="61"/>
@@ -14651,16 +14699,16 @@
         <f>U118+AB118+AI118+AP118+AW118</f>
         <v>0</v>
       </c>
-      <c r="AY118" s="293"/>
-      <c r="AZ118" s="291" t="s">
+      <c r="AY118" s="292"/>
+      <c r="AZ118" s="290" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="119" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A119" s="283"/>
       <c r="B119" s="284"/>
-      <c r="C119" s="294"/>
-      <c r="D119" s="295"/>
+      <c r="C119" s="293"/>
+      <c r="D119" s="294"/>
       <c r="E119" s="150">
         <f>SUM(E116:E118)</f>
         <v>0</v>
@@ -14682,13 +14730,13 @@
         <v>0</v>
       </c>
       <c r="J119" s="153">
-        <f>SUM(E119:I119)</f>
-        <v>0</v>
-      </c>
-      <c r="K119" s="296"/>
-      <c r="L119" s="297"/>
-      <c r="M119" s="298"/>
-      <c r="N119" s="299"/>
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K119" s="295"/>
+      <c r="L119" s="296"/>
+      <c r="M119" s="297"/>
+      <c r="N119" s="298"/>
       <c r="O119" s="80">
         <f t="shared" ref="O119" si="149">SUM(O116:O118)</f>
         <v>0</v>
@@ -14833,16 +14881,16 @@
         <f t="shared" si="150"/>
         <v>0</v>
       </c>
-      <c r="AY119" s="298"/>
-      <c r="AZ119" s="299"/>
+      <c r="AY119" s="297"/>
+      <c r="AZ119" s="298"/>
     </row>
     <row r="120" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A120" s="283"/>
       <c r="B120" s="284"/>
-      <c r="C120" s="300" t="s">
+      <c r="C120" s="299" t="s">
         <v>54</v>
       </c>
-      <c r="D120" s="301" t="s">
+      <c r="D120" s="300" t="s">
         <v>98</v>
       </c>
       <c r="E120" s="133">
@@ -14865,11 +14913,12 @@
         <f>AW120</f>
         <v>0</v>
       </c>
-      <c r="J120" s="287">
-        <v>0</v>
-      </c>
-      <c r="K120" s="288"/>
-      <c r="L120" s="289"/>
+      <c r="J120" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K120" s="287"/>
+      <c r="L120" s="288"/>
       <c r="M120" s="162" t="s">
         <v>54</v>
       </c>
@@ -14964,13 +15013,14 @@
         <f>AW121</f>
         <v>0</v>
       </c>
-      <c r="J121" s="287">
-        <v>0</v>
-      </c>
-      <c r="K121" s="288"/>
-      <c r="L121" s="289"/>
-      <c r="M121" s="290"/>
-      <c r="N121" s="291" t="s">
+      <c r="J121" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K121" s="287"/>
+      <c r="L121" s="288"/>
+      <c r="M121" s="289"/>
+      <c r="N121" s="290" t="s">
         <v>99</v>
       </c>
       <c r="O121" s="61"/>
@@ -15027,8 +15077,8 @@
         <f>U121+AB121+AI121+AP121+AW121</f>
         <v>0</v>
       </c>
-      <c r="AY121" s="290"/>
-      <c r="AZ121" s="291" t="s">
+      <c r="AY121" s="289"/>
+      <c r="AZ121" s="290" t="s">
         <v>99</v>
       </c>
     </row>
@@ -15059,15 +15109,16 @@
         <f>AW122</f>
         <v>0</v>
       </c>
-      <c r="J122" s="287">
-        <v>0</v>
-      </c>
-      <c r="K122" s="288"/>
-      <c r="L122" s="289"/>
-      <c r="M122" s="290" t="s">
+      <c r="J122" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K122" s="287"/>
+      <c r="L122" s="288"/>
+      <c r="M122" s="289" t="s">
         <v>103</v>
       </c>
-      <c r="N122" s="291" t="s">
+      <c r="N122" s="290" t="s">
         <v>107</v>
       </c>
       <c r="O122" s="61"/>
@@ -15124,17 +15175,17 @@
         <f>U122+AB122+AI122+AP122+AW122</f>
         <v>0</v>
       </c>
-      <c r="AY122" s="290" t="s">
+      <c r="AY122" s="289" t="s">
         <v>103</v>
       </c>
-      <c r="AZ122" s="291" t="s">
+      <c r="AZ122" s="290" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="123" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A123" s="283"/>
       <c r="B123" s="284"/>
-      <c r="C123" s="292"/>
+      <c r="C123" s="291"/>
       <c r="D123" s="286" t="s">
         <v>111</v>
       </c>
@@ -15156,15 +15207,16 @@
       </c>
       <c r="I123" s="135">
         <f>AW123</f>
-        <v>0</v>
-      </c>
-      <c r="J123" s="287">
-        <v>0</v>
-      </c>
-      <c r="K123" s="288"/>
-      <c r="L123" s="289"/>
-      <c r="M123" s="293"/>
-      <c r="N123" s="291" t="s">
+        <v>5.5</v>
+      </c>
+      <c r="J123" s="136">
+        <f t="shared" si="107"/>
+        <v>26.25</v>
+      </c>
+      <c r="K123" s="287"/>
+      <c r="L123" s="288"/>
+      <c r="M123" s="292"/>
+      <c r="N123" s="290" t="s">
         <v>111</v>
       </c>
       <c r="O123" s="61"/>
@@ -15230,28 +15282,35 @@
       </c>
       <c r="AQ123" s="61"/>
       <c r="AR123" s="141"/>
-      <c r="AS123" s="135"/>
-      <c r="AT123" s="135"/>
+      <c r="AS123" s="359">
+        <f>0.25+1.25+2.25</f>
+        <v>3.75</v>
+      </c>
+      <c r="AT123" s="135">
+        <v>0.75</v>
+      </c>
       <c r="AU123" s="135"/>
-      <c r="AV123" s="135"/>
+      <c r="AV123" s="135">
+        <v>1</v>
+      </c>
       <c r="AW123" s="142">
         <f>SUM(AR123:AV123)</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="AX123" s="65">
         <f>U123+AB123+AI123+AP123+AW123</f>
-        <v>20.75</v>
-      </c>
-      <c r="AY123" s="293"/>
-      <c r="AZ123" s="291" t="s">
+        <v>26.25</v>
+      </c>
+      <c r="AY123" s="292"/>
+      <c r="AZ123" s="290" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="124" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A124" s="283"/>
       <c r="B124" s="284"/>
-      <c r="C124" s="294"/>
-      <c r="D124" s="295"/>
+      <c r="C124" s="293"/>
+      <c r="D124" s="294"/>
       <c r="E124" s="150">
         <f>SUM(E120:E123)</f>
         <v>5.5</v>
@@ -15270,16 +15329,16 @@
       </c>
       <c r="I124" s="152">
         <f>SUM(I120:I123)</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="J124" s="153">
-        <f>SUM(E124:I124)</f>
-        <v>20.75</v>
-      </c>
-      <c r="K124" s="296"/>
-      <c r="L124" s="297"/>
-      <c r="M124" s="298"/>
-      <c r="N124" s="299"/>
+        <f t="shared" si="107"/>
+        <v>26.25</v>
+      </c>
+      <c r="K124" s="295"/>
+      <c r="L124" s="296"/>
+      <c r="M124" s="297"/>
+      <c r="N124" s="298"/>
       <c r="O124" s="80">
         <f t="shared" ref="O124" si="151">SUM(O120:O123)</f>
         <v>0</v>
@@ -15402,11 +15461,11 @@
       </c>
       <c r="AS124" s="80">
         <f t="shared" si="152"/>
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="AT124" s="80">
         <f t="shared" si="152"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AU124" s="80">
         <f t="shared" si="152"/>
@@ -15414,26 +15473,26 @@
       </c>
       <c r="AV124" s="80">
         <f t="shared" si="152"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW124" s="91">
         <f t="shared" si="152"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="AX124" s="92">
         <f t="shared" si="152"/>
-        <v>20.75</v>
-      </c>
-      <c r="AY124" s="298"/>
-      <c r="AZ124" s="299"/>
+        <v>26.25</v>
+      </c>
+      <c r="AY124" s="297"/>
+      <c r="AZ124" s="298"/>
     </row>
     <row r="125" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A125" s="283"/>
       <c r="B125" s="284"/>
-      <c r="C125" s="300" t="s">
+      <c r="C125" s="299" t="s">
         <v>57</v>
       </c>
-      <c r="D125" s="301" t="s">
+      <c r="D125" s="300" t="s">
         <v>100</v>
       </c>
       <c r="E125" s="133">
@@ -15456,11 +15515,12 @@
         <f>AW125</f>
         <v>0</v>
       </c>
-      <c r="J125" s="287">
-        <v>0</v>
-      </c>
-      <c r="K125" s="288"/>
-      <c r="L125" s="289"/>
+      <c r="J125" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K125" s="287"/>
+      <c r="L125" s="288"/>
       <c r="M125" s="162" t="s">
         <v>57</v>
       </c>
@@ -15555,13 +15615,14 @@
         <f>AW126</f>
         <v>0</v>
       </c>
-      <c r="J126" s="287">
-        <v>0</v>
-      </c>
-      <c r="K126" s="288"/>
-      <c r="L126" s="289"/>
-      <c r="M126" s="290"/>
-      <c r="N126" s="291" t="s">
+      <c r="J126" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K126" s="287"/>
+      <c r="L126" s="288"/>
+      <c r="M126" s="289"/>
+      <c r="N126" s="290" t="s">
         <v>101</v>
       </c>
       <c r="O126" s="61"/>
@@ -15618,15 +15679,15 @@
         <f>U126+AB126+AI126+AP126+AW126</f>
         <v>0</v>
       </c>
-      <c r="AY126" s="290"/>
-      <c r="AZ126" s="291" t="s">
+      <c r="AY126" s="289"/>
+      <c r="AZ126" s="290" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="127" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A127" s="283"/>
       <c r="B127" s="284"/>
-      <c r="C127" s="292"/>
+      <c r="C127" s="291"/>
       <c r="D127" s="286" t="s">
         <v>112</v>
       </c>
@@ -15650,13 +15711,14 @@
         <f>AW127</f>
         <v>0</v>
       </c>
-      <c r="J127" s="287">
-        <v>0</v>
-      </c>
-      <c r="K127" s="288"/>
-      <c r="L127" s="289"/>
-      <c r="M127" s="293"/>
-      <c r="N127" s="291" t="s">
+      <c r="J127" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K127" s="287"/>
+      <c r="L127" s="288"/>
+      <c r="M127" s="292"/>
+      <c r="N127" s="290" t="s">
         <v>112</v>
       </c>
       <c r="O127" s="61"/>
@@ -15713,16 +15775,16 @@
         <f>U127+AB127+AI127+AP127+AW127</f>
         <v>0</v>
       </c>
-      <c r="AY127" s="293"/>
-      <c r="AZ127" s="291" t="s">
+      <c r="AY127" s="292"/>
+      <c r="AZ127" s="290" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="128" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A128" s="283"/>
       <c r="B128" s="284"/>
-      <c r="C128" s="294"/>
-      <c r="D128" s="295"/>
+      <c r="C128" s="293"/>
+      <c r="D128" s="294"/>
       <c r="E128" s="150">
         <f>SUM(E125:E127)</f>
         <v>0</v>
@@ -15744,13 +15806,13 @@
         <v>0</v>
       </c>
       <c r="J128" s="153">
-        <f>SUM(E128:I128)</f>
-        <v>0</v>
-      </c>
-      <c r="K128" s="296"/>
-      <c r="L128" s="297"/>
-      <c r="M128" s="298"/>
-      <c r="N128" s="299"/>
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K128" s="295"/>
+      <c r="L128" s="296"/>
+      <c r="M128" s="297"/>
+      <c r="N128" s="298"/>
       <c r="O128" s="80">
         <f t="shared" ref="O128" si="153">SUM(O125:O127)</f>
         <v>0</v>
@@ -15895,16 +15957,16 @@
         <f t="shared" si="154"/>
         <v>0</v>
       </c>
-      <c r="AY128" s="298"/>
-      <c r="AZ128" s="299"/>
+      <c r="AY128" s="297"/>
+      <c r="AZ128" s="298"/>
     </row>
     <row r="129" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A129" s="283"/>
       <c r="B129" s="284"/>
-      <c r="C129" s="300" t="s">
+      <c r="C129" s="299" t="s">
         <v>102</v>
       </c>
-      <c r="D129" s="301" t="s">
+      <c r="D129" s="300" t="s">
         <v>114</v>
       </c>
       <c r="E129" s="133">
@@ -15925,13 +15987,14 @@
       </c>
       <c r="I129" s="135">
         <f>AW129</f>
-        <v>0</v>
-      </c>
-      <c r="J129" s="287">
-        <v>0</v>
-      </c>
-      <c r="K129" s="288"/>
-      <c r="L129" s="289" t="s">
+        <v>3.25</v>
+      </c>
+      <c r="J129" s="136">
+        <f t="shared" si="107"/>
+        <v>11.5</v>
+      </c>
+      <c r="K129" s="287"/>
+      <c r="L129" s="288" t="s">
         <v>124</v>
       </c>
       <c r="M129" s="162" t="s">
@@ -15989,16 +16052,23 @@
       <c r="AQ129" s="61"/>
       <c r="AR129" s="141"/>
       <c r="AS129" s="135"/>
-      <c r="AT129" s="135"/>
-      <c r="AU129" s="135"/>
-      <c r="AV129" s="135"/>
+      <c r="AT129" s="135">
+        <f>0.25+0.75+1</f>
+        <v>2</v>
+      </c>
+      <c r="AU129" s="135">
+        <v>0.25</v>
+      </c>
+      <c r="AV129" s="135">
+        <v>1</v>
+      </c>
       <c r="AW129" s="142">
         <f>SUM(AR129:AV129)</f>
-        <v>0</v>
+        <v>3.25</v>
       </c>
       <c r="AX129" s="65">
         <f>U129+AB129+AI129+AP129+AW129</f>
-        <v>8.25</v>
+        <v>11.5</v>
       </c>
       <c r="AY129" s="162" t="s">
         <v>102</v>
@@ -16034,11 +16104,12 @@
         <f t="shared" ref="I130:I131" si="159">AW130</f>
         <v>0</v>
       </c>
-      <c r="J130" s="287">
-        <v>0</v>
-      </c>
-      <c r="K130" s="288"/>
-      <c r="L130" s="289"/>
+      <c r="J130" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K130" s="287"/>
+      <c r="L130" s="288"/>
       <c r="M130" s="162" t="s">
         <v>117</v>
       </c>
@@ -16133,20 +16204,21 @@
       </c>
       <c r="I131" s="135">
         <f t="shared" si="159"/>
-        <v>5</v>
-      </c>
-      <c r="J131" s="287">
-        <v>0</v>
-      </c>
-      <c r="K131" s="288"/>
-      <c r="L131" s="289" t="s">
+        <v>7.75</v>
+      </c>
+      <c r="J131" s="136">
+        <f t="shared" si="107"/>
+        <v>14.75</v>
+      </c>
+      <c r="K131" s="287"/>
+      <c r="L131" s="288" t="s">
         <v>127</v>
       </c>
       <c r="M131" s="162" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="N131" s="163" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="O131" s="61"/>
       <c r="P131" s="141"/>
@@ -16195,16 +16267,20 @@
         <v>5</v>
       </c>
       <c r="AS131" s="135"/>
-      <c r="AT131" s="135"/>
-      <c r="AU131" s="135"/>
+      <c r="AT131" s="135">
+        <v>0.75</v>
+      </c>
+      <c r="AU131" s="135">
+        <v>2</v>
+      </c>
       <c r="AV131" s="135"/>
       <c r="AW131" s="142">
         <f t="shared" si="164"/>
-        <v>5</v>
+        <v>7.75</v>
       </c>
       <c r="AX131" s="65">
         <f t="shared" si="165"/>
-        <v>12</v>
+        <v>14.75</v>
       </c>
       <c r="AY131" s="162" t="s">
         <v>119</v>
@@ -16216,7 +16292,7 @@
     <row r="132" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A132" s="283"/>
       <c r="B132" s="284"/>
-      <c r="C132" s="302" t="s">
+      <c r="C132" s="301" t="s">
         <v>113</v>
       </c>
       <c r="D132" s="286" t="s">
@@ -16242,15 +16318,16 @@
         <f>AW132</f>
         <v>0</v>
       </c>
-      <c r="J132" s="287">
-        <v>0</v>
-      </c>
-      <c r="K132" s="288"/>
-      <c r="L132" s="289"/>
-      <c r="M132" s="303" t="s">
+      <c r="J132" s="136">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="K132" s="287"/>
+      <c r="L132" s="288"/>
+      <c r="M132" s="302" t="s">
         <v>113</v>
       </c>
-      <c r="N132" s="291" t="s">
+      <c r="N132" s="290" t="s">
         <v>106</v>
       </c>
       <c r="O132" s="61"/>
@@ -16307,18 +16384,18 @@
         <f>U132+AB132+AI132+AP132+AW132</f>
         <v>0</v>
       </c>
-      <c r="AY132" s="303" t="s">
+      <c r="AY132" s="302" t="s">
         <v>30</v>
       </c>
-      <c r="AZ132" s="291" t="s">
+      <c r="AZ132" s="290" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="133" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A133" s="283"/>
       <c r="B133" s="284"/>
-      <c r="C133" s="294"/>
-      <c r="D133" s="295"/>
+      <c r="C133" s="293"/>
+      <c r="D133" s="294"/>
       <c r="E133" s="150">
         <f>SUM(E129:E132)</f>
         <v>7</v>
@@ -16337,16 +16414,16 @@
       </c>
       <c r="I133" s="152">
         <f>SUM(I129:I132)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J133" s="153">
-        <f>SUM(E133:I133)</f>
-        <v>20.25</v>
-      </c>
-      <c r="K133" s="296"/>
-      <c r="L133" s="297"/>
-      <c r="M133" s="298"/>
-      <c r="N133" s="299"/>
+        <f t="shared" si="107"/>
+        <v>26.25</v>
+      </c>
+      <c r="K133" s="295"/>
+      <c r="L133" s="296"/>
+      <c r="M133" s="297"/>
+      <c r="N133" s="298"/>
       <c r="O133" s="80">
         <f t="shared" ref="O133:AX133" si="166">SUM(O129:O132)</f>
         <v>0</v>
@@ -16473,31 +16550,31 @@
       </c>
       <c r="AT133" s="80">
         <f t="shared" si="166"/>
-        <v>0</v>
+        <v>2.75</v>
       </c>
       <c r="AU133" s="80">
         <f t="shared" si="166"/>
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="AV133" s="80">
         <f t="shared" si="166"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW133" s="91">
         <f t="shared" si="166"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="AX133" s="92">
         <f t="shared" si="166"/>
-        <v>20.25</v>
+        <v>26.25</v>
       </c>
       <c r="AY133" s="158"/>
       <c r="AZ133" s="159"/>
     </row>
     <row r="134" spans="1:52" s="120" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="304"/>
+      <c r="A134" s="303"/>
       <c r="B134" s="271"/>
-      <c r="C134" s="305" t="s">
+      <c r="C134" s="304" t="s">
         <v>104</v>
       </c>
       <c r="D134" s="130"/>
@@ -16519,162 +16596,151 @@
       </c>
       <c r="I134" s="123">
         <f t="shared" si="167"/>
-        <v>5</v>
+        <v>16.75</v>
       </c>
       <c r="J134" s="123">
         <f t="shared" si="167"/>
-        <v>41.75</v>
+        <v>53.5</v>
       </c>
       <c r="K134" s="264"/>
       <c r="L134" s="130"/>
-      <c r="M134" s="306"/>
-      <c r="N134" s="307"/>
-      <c r="O134" s="308"/>
-      <c r="P134" s="309">
+      <c r="M134" s="305"/>
+      <c r="N134" s="306"/>
+      <c r="O134" s="307"/>
+      <c r="P134" s="308">
         <f t="shared" ref="P134:U134" si="168">P107+P111+P115+P119+P124+P128+P133+P103</f>
         <v>3</v>
       </c>
-      <c r="Q134" s="308">
+      <c r="Q134" s="307">
         <f t="shared" si="168"/>
         <v>0</v>
       </c>
-      <c r="R134" s="308">
+      <c r="R134" s="307">
         <f t="shared" si="168"/>
         <v>2</v>
       </c>
-      <c r="S134" s="308">
+      <c r="S134" s="307">
         <f t="shared" si="168"/>
         <v>0.5</v>
       </c>
-      <c r="T134" s="318">
+      <c r="T134" s="317">
         <f t="shared" si="168"/>
         <v>7</v>
       </c>
-      <c r="U134" s="310">
+      <c r="U134" s="309">
         <f t="shared" si="168"/>
         <v>12.5</v>
       </c>
-      <c r="V134" s="308"/>
-      <c r="W134" s="309">
+      <c r="V134" s="307"/>
+      <c r="W134" s="308">
         <f t="shared" ref="W134:AB134" si="169">W107+W111+W115+W119+W124+W128+W133+W103</f>
         <v>4</v>
       </c>
-      <c r="X134" s="308">
+      <c r="X134" s="307">
         <f t="shared" si="169"/>
         <v>8.25</v>
       </c>
-      <c r="Y134" s="308">
+      <c r="Y134" s="307">
         <f t="shared" si="169"/>
         <v>2.75</v>
       </c>
-      <c r="Z134" s="308">
+      <c r="Z134" s="307">
         <f t="shared" si="169"/>
         <v>0</v>
       </c>
-      <c r="AA134" s="318">
+      <c r="AA134" s="317">
         <f t="shared" si="169"/>
         <v>0</v>
       </c>
-      <c r="AB134" s="310">
+      <c r="AB134" s="309">
         <f t="shared" si="169"/>
         <v>15</v>
       </c>
-      <c r="AC134" s="308"/>
-      <c r="AD134" s="309">
+      <c r="AC134" s="307"/>
+      <c r="AD134" s="308">
         <f t="shared" ref="AD134:AI134" si="170">AD107+AD111+AD115+AD119+AD124+AD128+AD133+AD103</f>
         <v>0</v>
       </c>
-      <c r="AE134" s="308">
+      <c r="AE134" s="307">
         <f t="shared" si="170"/>
         <v>0</v>
       </c>
-      <c r="AF134" s="308">
+      <c r="AF134" s="307">
         <f t="shared" si="170"/>
         <v>0</v>
       </c>
-      <c r="AG134" s="308">
+      <c r="AG134" s="307">
         <f t="shared" si="170"/>
         <v>0</v>
       </c>
-      <c r="AH134" s="318">
+      <c r="AH134" s="317">
         <f t="shared" si="170"/>
         <v>0</v>
       </c>
-      <c r="AI134" s="310">
+      <c r="AI134" s="309">
         <f t="shared" si="170"/>
         <v>0</v>
       </c>
-      <c r="AJ134" s="308"/>
-      <c r="AK134" s="309">
+      <c r="AJ134" s="307"/>
+      <c r="AK134" s="308">
         <f t="shared" ref="AK134:AP134" si="171">AK107+AK111+AK115+AK119+AK124+AK128+AK133+AK103</f>
         <v>0</v>
       </c>
-      <c r="AL134" s="308">
+      <c r="AL134" s="307">
         <f t="shared" si="171"/>
         <v>4</v>
       </c>
-      <c r="AM134" s="308">
+      <c r="AM134" s="307">
         <f t="shared" si="171"/>
         <v>1.25</v>
       </c>
-      <c r="AN134" s="308">
+      <c r="AN134" s="307">
         <f t="shared" si="171"/>
         <v>1.75</v>
       </c>
-      <c r="AO134" s="318">
+      <c r="AO134" s="317">
         <f t="shared" si="171"/>
         <v>2.25</v>
       </c>
-      <c r="AP134" s="310">
+      <c r="AP134" s="309">
         <f t="shared" si="171"/>
         <v>9.25</v>
       </c>
-      <c r="AQ134" s="308"/>
-      <c r="AR134" s="309">
+      <c r="AQ134" s="307"/>
+      <c r="AR134" s="308">
         <f t="shared" ref="AR134:AW134" si="172">AR107+AR111+AR115+AR119+AR124+AR128+AR133+AR103</f>
         <v>5</v>
       </c>
-      <c r="AS134" s="308">
+      <c r="AS134" s="307">
         <f t="shared" si="172"/>
-        <v>0</v>
-      </c>
-      <c r="AT134" s="308">
+        <v>3.75</v>
+      </c>
+      <c r="AT134" s="307">
         <f t="shared" si="172"/>
-        <v>0</v>
-      </c>
-      <c r="AU134" s="308">
+        <v>3.5</v>
+      </c>
+      <c r="AU134" s="307">
         <f t="shared" si="172"/>
-        <v>0</v>
-      </c>
-      <c r="AV134" s="318">
+        <v>2.5</v>
+      </c>
+      <c r="AV134" s="317">
         <f t="shared" si="172"/>
-        <v>0</v>
-      </c>
-      <c r="AW134" s="310">
+        <v>2</v>
+      </c>
+      <c r="AW134" s="309">
         <f t="shared" si="172"/>
-        <v>5</v>
-      </c>
-      <c r="AX134" s="308"/>
-      <c r="AY134" s="311"/>
-      <c r="AZ134" s="312"/>
+        <v>16.75</v>
+      </c>
+      <c r="AX134" s="307"/>
+      <c r="AY134" s="310"/>
+      <c r="AZ134" s="311"/>
     </row>
     <row r="137" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="E137" s="319"/>
-      <c r="U137" s="319"/>
+      <c r="E137" s="318"/>
+      <c r="U137" s="318"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AD3:AH3"/>
-    <mergeCell ref="W3:AA3"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="AR2:AV2"/>
-    <mergeCell ref="AK2:AO2"/>
-    <mergeCell ref="AD2:AH2"/>
-    <mergeCell ref="W2:AA2"/>
-    <mergeCell ref="P2:T2"/>
     <mergeCell ref="AY69:AZ69"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="AY101:AZ101"/>
@@ -16691,6 +16757,17 @@
     <mergeCell ref="AY28:AZ28"/>
     <mergeCell ref="AY37:AZ37"/>
     <mergeCell ref="AY63:AZ63"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AD3:AH3"/>
+    <mergeCell ref="W3:AA3"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="AR2:AV2"/>
+    <mergeCell ref="AK2:AO2"/>
+    <mergeCell ref="AD2:AH2"/>
+    <mergeCell ref="W2:AA2"/>
+    <mergeCell ref="P2:T2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>